<commit_message>
Cleaned up clint estimation
</commit_message>
<xml_diff>
--- a/working/KreutzPFAS/KreutzPFAS-Clint-Level4.xlsx
+++ b/working/KreutzPFAS/KreutzPFAS-Clint-Level4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\invitrotkstats\working\KreutzPFAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8221526-686C-491D-9533-DC490B24DF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6727786F-EF2C-461C-9F0E-F36B5B9EF677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="29940" yWindow="1140" windowWidth="24240" windowHeight="14715"/>
   </bookViews>
   <sheets>
     <sheet name="KreutzPFAS-Clint-Level4" sheetId="1" r:id="rId1"/>
@@ -67,12 +67,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Bis(1H,1H-perfluoropropyl)amine</t>
-  </si>
-  <si>
-    <t>DTXSID50381992</t>
-  </si>
-  <si>
     <t>1H,1H,8H,8H-Perfluoro-3,6-dioxaoctane-1,8-diol</t>
   </si>
   <si>
@@ -109,30 +103,36 @@
     <t>DTXSID90190949</t>
   </si>
   <si>
+    <t>Pentafluoropropionamide</t>
+  </si>
+  <si>
+    <t>DTXSID0059871</t>
+  </si>
+  <si>
+    <t>N-Methyl-N-trimethylsilylheptafluorobutyramide</t>
+  </si>
+  <si>
+    <t>DTXSID40379666</t>
+  </si>
+  <si>
+    <t>Heptafluorobutyramide</t>
+  </si>
+  <si>
+    <t>DTXSID2060965</t>
+  </si>
+  <si>
+    <t>Nonafluoropentanamide</t>
+  </si>
+  <si>
+    <t>DTXSID60400587</t>
+  </si>
+  <si>
     <t>1H,1H,5H-Perfluoropentanol</t>
   </si>
   <si>
     <t>DTXSID0059879</t>
   </si>
   <si>
-    <t>Pentafluoropropionamide</t>
-  </si>
-  <si>
-    <t>DTXSID0059871</t>
-  </si>
-  <si>
-    <t>Heptafluorobutyramide</t>
-  </si>
-  <si>
-    <t>DTXSID2060965</t>
-  </si>
-  <si>
-    <t>Nonafluoropentanamide</t>
-  </si>
-  <si>
-    <t>DTXSID60400587</t>
-  </si>
-  <si>
     <t>Perfluoropentanamide</t>
   </si>
   <si>
@@ -145,12 +145,6 @@
     <t>DTXSID80310730</t>
   </si>
   <si>
-    <t>N-Methyl-N-trimethylsilylheptafluorobutyramide</t>
-  </si>
-  <si>
-    <t>DTXSID40379666</t>
-  </si>
-  <si>
     <t>Dodecafluoroheptanol</t>
   </si>
   <si>
@@ -209,6 +203,12 @@
   </si>
   <si>
     <t>DTXSID70880230</t>
+  </si>
+  <si>
+    <t>4:2 Fluorotelomer alcohol</t>
+  </si>
+  <si>
+    <t>DTXSID1062122</t>
   </si>
 </sst>
 </file>
@@ -351,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,6 +529,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -692,9 +704,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1074,23 +1087,23 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L26"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" customWidth="1"/>
-    <col min="11" max="11" width="11.6328125" customWidth="1"/>
-    <col min="12" max="12" width="16.7265625" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" customWidth="1"/>
+    <col min="10" max="10" width="13.36328125" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -1142,13 +1155,13 @@
         <v>745</v>
       </c>
       <c r="D2">
-        <v>21.5</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>19.399999999999999</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>23.6</v>
+        <v>0</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -1160,13 +1173,13 @@
         <v>14</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>0.997</v>
       </c>
       <c r="K2">
         <v>0.752</v>
       </c>
-      <c r="L2">
-        <v>0.998</v>
+      <c r="L2" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -1177,16 +1190,16 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>959</v>
+        <v>949</v>
       </c>
       <c r="D3">
-        <v>667</v>
+        <v>6.97</v>
       </c>
       <c r="E3">
-        <v>667</v>
+        <v>6.03</v>
       </c>
       <c r="F3">
-        <v>667</v>
+        <v>7.83</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -1201,10 +1214,10 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0.752</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
+        <v>0.75</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -1214,17 +1227,17 @@
       <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4">
-        <v>949</v>
+      <c r="C4" t="s">
+        <v>17</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>13.9</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>10.3</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>17.2</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -1236,13 +1249,13 @@
         <v>14</v>
       </c>
       <c r="J4">
-        <v>0.98799999999999999</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>0.746</v>
-      </c>
-      <c r="L4">
-        <v>0.95</v>
+        <v>0.748</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.51200000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -1252,8 +1265,8 @@
       <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
+      <c r="C5">
+        <v>30503</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1262,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>3.77</v>
+        <v>175</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -1274,13 +1287,13 @@
         <v>14</v>
       </c>
       <c r="J5">
-        <v>0.75900000000000001</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="K5">
         <v>0.751</v>
       </c>
-      <c r="L5">
-        <v>0.96099999999999997</v>
+      <c r="L5" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -1291,16 +1304,16 @@
         <v>22</v>
       </c>
       <c r="C6">
-        <v>30503</v>
+        <v>30507</v>
       </c>
       <c r="D6">
-        <v>132</v>
+        <v>333</v>
       </c>
       <c r="E6">
-        <v>87.7</v>
+        <v>331</v>
       </c>
       <c r="F6">
-        <v>208</v>
+        <v>333</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
@@ -1315,10 +1328,10 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0.75</v>
-      </c>
-      <c r="L6">
-        <v>0.98</v>
+        <v>0.748</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -1329,16 +1342,16 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>30507</v>
+        <v>30516</v>
       </c>
       <c r="D7">
-        <v>667</v>
+        <v>76</v>
       </c>
       <c r="E7">
-        <v>667</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>667</v>
+        <v>208</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -1350,12 +1363,12 @@
         <v>14</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>0.41199999999999998</v>
       </c>
       <c r="K7">
-        <v>0.752</v>
-      </c>
-      <c r="L7">
+        <v>0.75</v>
+      </c>
+      <c r="L7" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1367,16 +1380,16 @@
         <v>26</v>
       </c>
       <c r="C8">
-        <v>30516</v>
+        <v>30501</v>
       </c>
       <c r="D8">
-        <v>198</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>177</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>220</v>
+        <v>55.7</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
@@ -1388,13 +1401,13 @@
         <v>14</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="K8">
-        <v>0.748</v>
-      </c>
-      <c r="L8">
-        <v>0.96399999999999997</v>
+        <v>0.755</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1405,16 +1418,16 @@
         <v>28</v>
       </c>
       <c r="C9">
-        <v>30501</v>
+        <v>273</v>
       </c>
       <c r="D9">
-        <v>62.7</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>22.4</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>77</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
@@ -1426,13 +1439,13 @@
         <v>14</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="K9">
-        <v>0.749</v>
-      </c>
-      <c r="L9">
-        <v>0.99099999999999999</v>
+        <v>0.753</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0.28100000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -1443,16 +1456,16 @@
         <v>30</v>
       </c>
       <c r="C10">
-        <v>900</v>
+        <v>476</v>
       </c>
       <c r="D10">
-        <v>15.6</v>
+        <v>25.7</v>
       </c>
       <c r="E10">
-        <v>14.2</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>16.899999999999999</v>
+        <v>314</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
@@ -1464,13 +1477,13 @@
         <v>14</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="K10">
-        <v>0.749</v>
-      </c>
-      <c r="L10">
-        <v>0.997</v>
+        <v>0.752</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.92100000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -1481,16 +1494,16 @@
         <v>32</v>
       </c>
       <c r="C11">
-        <v>273</v>
+        <v>908</v>
       </c>
       <c r="D11">
-        <v>4.13</v>
+        <v>14.7</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>11.8</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>16.7</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
@@ -1502,13 +1515,13 @@
         <v>14</v>
       </c>
       <c r="J11">
-        <v>0.23499999999999999</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="K11">
-        <v>0.752</v>
-      </c>
-      <c r="L11">
-        <v>0.98799999999999999</v>
+        <v>0.751</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.98199999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
@@ -1519,16 +1532,16 @@
         <v>34</v>
       </c>
       <c r="C12">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="D12">
-        <v>7.07</v>
+        <v>132</v>
       </c>
       <c r="E12">
-        <v>4.67</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>9.4</v>
+        <v>160</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
@@ -1540,13 +1553,13 @@
         <v>14</v>
       </c>
       <c r="J12">
-        <v>8.5999999999999998E-4</v>
+        <v>5.4600000000000003E-2</v>
       </c>
       <c r="K12">
-        <v>0.747</v>
-      </c>
-      <c r="L12">
-        <v>0.998</v>
+        <v>0.752</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.92400000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -1557,16 +1570,16 @@
         <v>36</v>
       </c>
       <c r="C13">
-        <v>909</v>
+        <v>900</v>
       </c>
       <c r="D13">
-        <v>16.100000000000001</v>
+        <v>3.73</v>
       </c>
       <c r="E13">
-        <v>13.9</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>18.2</v>
+        <v>6.1</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
@@ -1578,13 +1591,13 @@
         <v>14</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>0.122</v>
       </c>
       <c r="K13">
-        <v>0.746</v>
-      </c>
-      <c r="L13">
-        <v>0.999</v>
+        <v>0.749</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
@@ -1598,13 +1611,13 @@
         <v>916</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>14.8</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="F14">
-        <v>2.02</v>
+        <v>17.5</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
@@ -1616,13 +1629,13 @@
         <v>14</v>
       </c>
       <c r="J14">
-        <v>0.95699999999999996</v>
+        <v>0</v>
       </c>
       <c r="K14">
-        <v>0.751</v>
-      </c>
-      <c r="L14">
-        <v>0.95099999999999996</v>
+        <v>0.75</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.997</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -1636,13 +1649,13 @@
         <v>923</v>
       </c>
       <c r="D15">
-        <v>8.67</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>6.33</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>10.7</v>
+        <v>0</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
@@ -1654,13 +1667,13 @@
         <v>14</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="K15">
-        <v>0.747</v>
-      </c>
-      <c r="L15">
-        <v>0.997</v>
+        <v>0.749</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1.66E-3</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -1671,16 +1684,16 @@
         <v>42</v>
       </c>
       <c r="C16">
-        <v>476</v>
+        <v>906</v>
       </c>
       <c r="D16">
-        <v>22.3</v>
+        <v>176</v>
       </c>
       <c r="E16">
-        <v>20.7</v>
+        <v>167</v>
       </c>
       <c r="F16">
-        <v>24</v>
+        <v>185</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
@@ -1695,10 +1708,10 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>0.752</v>
-      </c>
-      <c r="L16">
-        <v>0.998</v>
+        <v>0.751</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
@@ -1709,16 +1722,16 @@
         <v>44</v>
       </c>
       <c r="C17">
-        <v>906</v>
+        <v>913</v>
       </c>
       <c r="D17">
-        <v>35.700000000000003</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="E17">
-        <v>34</v>
+        <v>6.63</v>
       </c>
       <c r="F17">
-        <v>37.299999999999997</v>
+        <v>11.9</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
@@ -1730,13 +1743,13 @@
         <v>14</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>3.6000000000000002E-4</v>
       </c>
       <c r="K17">
-        <v>0.751</v>
-      </c>
-      <c r="L17">
-        <v>0.999</v>
+        <v>0.752</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0.97899999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
@@ -1747,16 +1760,16 @@
         <v>46</v>
       </c>
       <c r="C18">
-        <v>913</v>
+        <v>965</v>
       </c>
       <c r="D18">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>2.66</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>6.3</v>
+        <v>76</v>
       </c>
       <c r="G18" t="s">
         <v>14</v>
@@ -1768,13 +1781,13 @@
         <v>14</v>
       </c>
       <c r="J18">
-        <v>1.8000000000000001E-4</v>
+        <v>0.79600000000000004</v>
       </c>
       <c r="K18">
-        <v>0.751</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
+        <v>0.75</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
@@ -1785,16 +1798,16 @@
         <v>48</v>
       </c>
       <c r="C19">
-        <v>965</v>
+        <v>477</v>
       </c>
       <c r="D19">
-        <v>38.299999999999997</v>
+        <v>20.9</v>
       </c>
       <c r="E19">
-        <v>36.700000000000003</v>
+        <v>15.2</v>
       </c>
       <c r="F19">
-        <v>40</v>
+        <v>25.1</v>
       </c>
       <c r="G19" t="s">
         <v>14</v>
@@ -1809,10 +1822,10 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>0.747</v>
-      </c>
-      <c r="L19">
-        <v>0.99399999999999999</v>
+        <v>0.75</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.93799999999999994</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
@@ -1823,16 +1836,16 @@
         <v>50</v>
       </c>
       <c r="C20">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D20">
-        <v>7.73</v>
+        <v>14.7</v>
       </c>
       <c r="E20">
-        <v>5.73</v>
+        <v>9</v>
       </c>
       <c r="F20">
-        <v>9.73</v>
+        <v>19.3</v>
       </c>
       <c r="G20" t="s">
         <v>14</v>
@@ -1844,13 +1857,13 @@
         <v>14</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>8.1999999999999998E-4</v>
       </c>
       <c r="K20">
         <v>0.75</v>
       </c>
-      <c r="L20">
-        <v>0.999</v>
+      <c r="L20" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -1861,16 +1874,16 @@
         <v>52</v>
       </c>
       <c r="C21">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="D21">
-        <v>2.83</v>
+        <v>22.9</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>15.4</v>
       </c>
       <c r="F21">
-        <v>5.4</v>
+        <v>28.2</v>
       </c>
       <c r="G21" t="s">
         <v>14</v>
@@ -1882,13 +1895,13 @@
         <v>14</v>
       </c>
       <c r="J21">
-        <v>0.35599999999999998</v>
+        <v>3.2000000000000003E-4</v>
       </c>
       <c r="K21">
-        <v>0.75</v>
-      </c>
-      <c r="L21">
-        <v>0.98299999999999998</v>
+        <v>0.749</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.999</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -1899,16 +1912,16 @@
         <v>54</v>
       </c>
       <c r="C22">
-        <v>464</v>
+        <v>945</v>
       </c>
       <c r="D22">
-        <v>5.03</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>3.09</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>6.87</v>
+        <v>0</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
@@ -1919,14 +1932,14 @@
       <c r="I22" t="s">
         <v>14</v>
       </c>
-      <c r="J22" s="1">
-        <v>8.0000000000000007E-5</v>
+      <c r="J22">
+        <v>0.97499999999999998</v>
       </c>
       <c r="K22">
-        <v>0.751</v>
-      </c>
-      <c r="L22">
-        <v>0.999</v>
+        <v>0.748</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.97899999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
@@ -1937,16 +1950,16 @@
         <v>56</v>
       </c>
       <c r="C23">
-        <v>945</v>
+        <v>274</v>
       </c>
       <c r="D23">
-        <v>1.88</v>
+        <v>106</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="F23">
-        <v>5.23</v>
+        <v>116</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
@@ -1958,13 +1971,13 @@
         <v>14</v>
       </c>
       <c r="J23">
-        <v>0.46100000000000002</v>
+        <v>0</v>
       </c>
       <c r="K23">
         <v>0.752</v>
       </c>
-      <c r="L23">
-        <v>0.97699999999999998</v>
+      <c r="L23" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
@@ -1975,16 +1988,16 @@
         <v>58</v>
       </c>
       <c r="C24">
-        <v>274</v>
+        <v>474</v>
       </c>
       <c r="D24">
-        <v>85</v>
+        <v>7.33</v>
       </c>
       <c r="E24">
-        <v>52.7</v>
+        <v>4.7</v>
       </c>
       <c r="F24">
-        <v>151</v>
+        <v>11.4</v>
       </c>
       <c r="G24" t="s">
         <v>14</v>
@@ -1999,10 +2012,10 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <v>0.75</v>
-      </c>
-      <c r="L24">
-        <v>0.98599999999999999</v>
+        <v>0.749</v>
+      </c>
+      <c r="L24" s="1">
+        <v>2.1399999999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -2013,16 +2026,16 @@
         <v>60</v>
       </c>
       <c r="C25">
-        <v>474</v>
+        <v>3096</v>
       </c>
       <c r="D25">
-        <v>11.2</v>
+        <v>327</v>
       </c>
       <c r="E25">
-        <v>9.0299999999999994</v>
+        <v>299</v>
       </c>
       <c r="F25">
-        <v>13.1</v>
+        <v>333</v>
       </c>
       <c r="G25" t="s">
         <v>14</v>
@@ -2037,10 +2050,10 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>0.754</v>
-      </c>
-      <c r="L25">
-        <v>0.998</v>
+        <v>0.749</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
@@ -2051,16 +2064,16 @@
         <v>62</v>
       </c>
       <c r="C26">
-        <v>3096</v>
+        <v>971</v>
       </c>
       <c r="D26">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="E26">
-        <v>241</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>567</v>
+        <v>332</v>
       </c>
       <c r="G26" t="s">
         <v>14</v>
@@ -2072,13 +2085,13 @@
         <v>14</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>3.9899999999999998E-2</v>
       </c>
       <c r="K26">
-        <v>0.752</v>
+        <v>0.748</v>
       </c>
       <c r="L26">
-        <v>0.72599999999999998</v>
+        <v>0.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added stability test to UC, harmonized the three Bayesian functions
</commit_message>
<xml_diff>
--- a/working/KreutzPFAS/KreutzPFAS-Clint-Level4.xlsx
+++ b/working/KreutzPFAS/KreutzPFAS-Clint-Level4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\invitrotkstats\working\KreutzPFAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6727786F-EF2C-461C-9F0E-F36B5B9EF677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4601CE4F-2AAD-4DFF-8100-A09359283AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="1140" windowWidth="24240" windowHeight="14715"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="KreutzPFAS-Clint-Level4" sheetId="1" r:id="rId1"/>
@@ -103,46 +103,46 @@
     <t>DTXSID90190949</t>
   </si>
   <si>
+    <t>1H,1H,5H-Perfluoropentanol</t>
+  </si>
+  <si>
+    <t>DTXSID0059879</t>
+  </si>
+  <si>
     <t>Pentafluoropropionamide</t>
   </si>
   <si>
     <t>DTXSID0059871</t>
   </si>
   <si>
+    <t>Heptafluorobutyramide</t>
+  </si>
+  <si>
+    <t>DTXSID2060965</t>
+  </si>
+  <si>
+    <t>Nonafluoropentanamide</t>
+  </si>
+  <si>
+    <t>DTXSID60400587</t>
+  </si>
+  <si>
+    <t>Perfluoropentanamide</t>
+  </si>
+  <si>
+    <t>DTXSID70366226</t>
+  </si>
+  <si>
+    <t>Octafluoroadipamide</t>
+  </si>
+  <si>
+    <t>DTXSID80310730</t>
+  </si>
+  <si>
     <t>N-Methyl-N-trimethylsilylheptafluorobutyramide</t>
   </si>
   <si>
     <t>DTXSID40379666</t>
-  </si>
-  <si>
-    <t>Heptafluorobutyramide</t>
-  </si>
-  <si>
-    <t>DTXSID2060965</t>
-  </si>
-  <si>
-    <t>Nonafluoropentanamide</t>
-  </si>
-  <si>
-    <t>DTXSID60400587</t>
-  </si>
-  <si>
-    <t>1H,1H,5H-Perfluoropentanol</t>
-  </si>
-  <si>
-    <t>DTXSID0059879</t>
-  </si>
-  <si>
-    <t>Perfluoropentanamide</t>
-  </si>
-  <si>
-    <t>DTXSID70366226</t>
-  </si>
-  <si>
-    <t>Octafluoroadipamide</t>
-  </si>
-  <si>
-    <t>DTXSID80310730</t>
   </si>
   <si>
     <t>Dodecafluoroheptanol</t>
@@ -351,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,18 +529,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -704,10 +692,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1087,7 +1073,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1173,12 +1159,12 @@
         <v>14</v>
       </c>
       <c r="J2">
-        <v>0.997</v>
+        <v>0.996</v>
       </c>
       <c r="K2">
         <v>0.752</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2">
         <v>0</v>
       </c>
     </row>
@@ -1193,13 +1179,13 @@
         <v>949</v>
       </c>
       <c r="D3">
-        <v>6.97</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>6.03</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>7.83</v>
+        <v>2.94</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -1211,13 +1197,13 @@
         <v>14</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="K3">
-        <v>0.75</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1</v>
+        <v>0.749</v>
+      </c>
+      <c r="L3">
+        <v>0.999</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -1231,13 +1217,13 @@
         <v>17</v>
       </c>
       <c r="D4">
-        <v>13.9</v>
+        <v>14.7</v>
       </c>
       <c r="E4">
-        <v>10.3</v>
+        <v>11.5</v>
       </c>
       <c r="F4">
-        <v>17.2</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -1252,10 +1238,10 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0.748</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0.51200000000000001</v>
+        <v>0.753</v>
+      </c>
+      <c r="L4">
+        <v>0.97899999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -1275,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -1287,12 +1273,12 @@
         <v>14</v>
       </c>
       <c r="J5">
-        <v>0.65500000000000003</v>
+        <v>0.69099999999999995</v>
       </c>
       <c r="K5">
-        <v>0.751</v>
-      </c>
-      <c r="L5" s="1">
+        <v>0.749</v>
+      </c>
+      <c r="L5">
         <v>0</v>
       </c>
     </row>
@@ -1307,13 +1293,13 @@
         <v>30507</v>
       </c>
       <c r="D6">
-        <v>333</v>
+        <v>141</v>
       </c>
       <c r="E6">
-        <v>331</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>333</v>
+        <v>281</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
@@ -1325,12 +1311,12 @@
         <v>14</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="K6">
-        <v>0.748</v>
-      </c>
-      <c r="L6" s="1">
+        <v>0.749</v>
+      </c>
+      <c r="L6">
         <v>0</v>
       </c>
     </row>
@@ -1345,13 +1331,13 @@
         <v>30516</v>
       </c>
       <c r="D7">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>208</v>
+        <v>169</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -1363,12 +1349,12 @@
         <v>14</v>
       </c>
       <c r="J7">
-        <v>0.41199999999999998</v>
+        <v>0.27100000000000002</v>
       </c>
       <c r="K7">
-        <v>0.75</v>
-      </c>
-      <c r="L7" s="1">
+        <v>0.748</v>
+      </c>
+      <c r="L7">
         <v>0</v>
       </c>
     </row>
@@ -1383,13 +1369,13 @@
         <v>30501</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>27.3</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>21.2</v>
       </c>
       <c r="F8">
-        <v>55.7</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
@@ -1401,12 +1387,12 @@
         <v>14</v>
       </c>
       <c r="J8">
-        <v>0.57999999999999996</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>0.755</v>
-      </c>
-      <c r="L8" s="1">
+        <v>0.753</v>
+      </c>
+      <c r="L8">
         <v>0</v>
       </c>
     </row>
@@ -1418,16 +1404,16 @@
         <v>28</v>
       </c>
       <c r="C9">
-        <v>273</v>
+        <v>900</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>3.83</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>9.6300000000000008</v>
+        <v>6.07</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
@@ -1439,13 +1425,13 @@
         <v>14</v>
       </c>
       <c r="J9">
-        <v>0.71799999999999997</v>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="K9">
-        <v>0.753</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0.28100000000000003</v>
+        <v>0.751</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -1456,16 +1442,16 @@
         <v>30</v>
       </c>
       <c r="C10">
-        <v>476</v>
+        <v>273</v>
       </c>
       <c r="D10">
-        <v>25.7</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>314</v>
+        <v>5.37</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
@@ -1477,13 +1463,13 @@
         <v>14</v>
       </c>
       <c r="J10">
-        <v>5.1999999999999998E-2</v>
+        <v>0.82299999999999995</v>
       </c>
       <c r="K10">
-        <v>0.752</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0.92100000000000004</v>
+        <v>0.748</v>
+      </c>
+      <c r="L10">
+        <v>0.94299999999999995</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -1497,13 +1483,13 @@
         <v>908</v>
       </c>
       <c r="D11">
-        <v>14.7</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>11.8</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>16.7</v>
+        <v>0</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
@@ -1515,13 +1501,13 @@
         <v>14</v>
       </c>
       <c r="J11">
-        <v>1.6199999999999999E-2</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="K11">
-        <v>0.751</v>
-      </c>
-      <c r="L11" s="1">
-        <v>0.98199999999999998</v>
+        <v>0.748</v>
+      </c>
+      <c r="L11">
+        <v>7.1599999999999997E-3</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
@@ -1535,13 +1521,13 @@
         <v>909</v>
       </c>
       <c r="D12">
-        <v>132</v>
+        <v>88.7</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>62.7</v>
       </c>
       <c r="F12">
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
@@ -1553,13 +1539,13 @@
         <v>14</v>
       </c>
       <c r="J12">
-        <v>5.4600000000000003E-2</v>
+        <v>5.6800000000000002E-3</v>
       </c>
       <c r="K12">
-        <v>0.752</v>
-      </c>
-      <c r="L12" s="1">
-        <v>0.92400000000000004</v>
+        <v>0.75</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -1570,16 +1556,16 @@
         <v>36</v>
       </c>
       <c r="C13">
-        <v>900</v>
+        <v>916</v>
       </c>
       <c r="D13">
-        <v>3.73</v>
+        <v>0</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>6.1</v>
+        <v>3.04</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
@@ -1591,13 +1577,13 @@
         <v>14</v>
       </c>
       <c r="J13">
-        <v>0.122</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="K13">
-        <v>0.749</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0</v>
+        <v>0.748</v>
+      </c>
+      <c r="L13">
+        <v>0.99299999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
@@ -1608,16 +1594,16 @@
         <v>38</v>
       </c>
       <c r="C14">
-        <v>916</v>
+        <v>923</v>
       </c>
       <c r="D14">
-        <v>14.8</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>11.5</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>17.5</v>
+        <v>0</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
@@ -1629,13 +1615,13 @@
         <v>14</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>0.995</v>
       </c>
       <c r="K14">
-        <v>0.75</v>
-      </c>
-      <c r="L14" s="1">
-        <v>0.997</v>
+        <v>0.748</v>
+      </c>
+      <c r="L14">
+        <v>7.2000000000000005E-4</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -1646,16 +1632,16 @@
         <v>40</v>
       </c>
       <c r="C15">
-        <v>923</v>
+        <v>476</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>6.1</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>17.2</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
@@ -1667,13 +1653,13 @@
         <v>14</v>
       </c>
       <c r="J15">
-        <v>0.99299999999999999</v>
+        <v>0.159</v>
       </c>
       <c r="K15">
-        <v>0.749</v>
-      </c>
-      <c r="L15" s="2">
-        <v>1.66E-3</v>
+        <v>0.747</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -1687,13 +1673,13 @@
         <v>906</v>
       </c>
       <c r="D16">
-        <v>176</v>
+        <v>93.3</v>
       </c>
       <c r="E16">
-        <v>167</v>
+        <v>81.7</v>
       </c>
       <c r="F16">
-        <v>185</v>
+        <v>104</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
@@ -1708,9 +1694,9 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>0.751</v>
-      </c>
-      <c r="L16" s="1">
+        <v>0.748</v>
+      </c>
+      <c r="L16">
         <v>0</v>
       </c>
     </row>
@@ -1725,13 +1711,13 @@
         <v>913</v>
       </c>
       <c r="D17">
-        <v>9.5299999999999994</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E17">
-        <v>6.63</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>11.9</v>
+        <v>6.57</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
@@ -1743,13 +1729,13 @@
         <v>14</v>
       </c>
       <c r="J17">
-        <v>3.6000000000000002E-4</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="K17">
-        <v>0.752</v>
-      </c>
-      <c r="L17" s="1">
-        <v>0.97899999999999998</v>
+        <v>0.75</v>
+      </c>
+      <c r="L17">
+        <v>0.73499999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
@@ -1769,7 +1755,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>76</v>
+        <v>77.3</v>
       </c>
       <c r="G18" t="s">
         <v>14</v>
@@ -1781,12 +1767,12 @@
         <v>14</v>
       </c>
       <c r="J18">
-        <v>0.79600000000000004</v>
+        <v>0.72199999999999998</v>
       </c>
       <c r="K18">
-        <v>0.75</v>
-      </c>
-      <c r="L18" s="1">
+        <v>0.752</v>
+      </c>
+      <c r="L18">
         <v>0</v>
       </c>
     </row>
@@ -1801,13 +1787,13 @@
         <v>477</v>
       </c>
       <c r="D19">
-        <v>20.9</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>15.2</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>25.1</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
         <v>14</v>
@@ -1819,13 +1805,13 @@
         <v>14</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>0.873</v>
       </c>
       <c r="K19">
-        <v>0.75</v>
-      </c>
-      <c r="L19" s="1">
-        <v>0.93799999999999994</v>
+        <v>0.748</v>
+      </c>
+      <c r="L19">
+        <v>0.09</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
@@ -1839,13 +1825,13 @@
         <v>479</v>
       </c>
       <c r="D20">
-        <v>14.7</v>
+        <v>5.03</v>
       </c>
       <c r="E20">
-        <v>9</v>
+        <v>2.11</v>
       </c>
       <c r="F20">
-        <v>19.3</v>
+        <v>7.3</v>
       </c>
       <c r="G20" t="s">
         <v>14</v>
@@ -1857,13 +1843,13 @@
         <v>14</v>
       </c>
       <c r="J20">
-        <v>8.1999999999999998E-4</v>
+        <v>1.5599999999999999E-2</v>
       </c>
       <c r="K20">
         <v>0.75</v>
       </c>
-      <c r="L20" s="1">
-        <v>1</v>
+      <c r="L20">
+        <v>0.996</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -1877,13 +1863,13 @@
         <v>464</v>
       </c>
       <c r="D21">
-        <v>22.9</v>
+        <v>5.23</v>
       </c>
       <c r="E21">
-        <v>15.4</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>28.2</v>
+        <v>7.23</v>
       </c>
       <c r="G21" t="s">
         <v>14</v>
@@ -1895,13 +1881,13 @@
         <v>14</v>
       </c>
       <c r="J21">
-        <v>3.2000000000000003E-4</v>
+        <v>3.32E-2</v>
       </c>
       <c r="K21">
-        <v>0.749</v>
-      </c>
-      <c r="L21" s="1">
-        <v>0.999</v>
+        <v>0.752</v>
+      </c>
+      <c r="L21">
+        <v>0.96699999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -1921,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>4.07</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
@@ -1933,13 +1919,13 @@
         <v>14</v>
       </c>
       <c r="J22">
-        <v>0.97499999999999998</v>
+        <v>0.86399999999999999</v>
       </c>
       <c r="K22">
-        <v>0.748</v>
-      </c>
-      <c r="L22" s="1">
-        <v>0.97899999999999998</v>
+        <v>0.751</v>
+      </c>
+      <c r="L22">
+        <v>0.81599999999999995</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
@@ -1953,13 +1939,13 @@
         <v>274</v>
       </c>
       <c r="D23">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E23">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F23">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
@@ -1974,10 +1960,10 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>0.752</v>
-      </c>
-      <c r="L23" s="2">
-        <v>0</v>
+        <v>0.748</v>
+      </c>
+      <c r="L23">
+        <v>2.06E-2</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
@@ -1991,13 +1977,13 @@
         <v>474</v>
       </c>
       <c r="D24">
-        <v>7.33</v>
+        <v>7.4</v>
       </c>
       <c r="E24">
-        <v>4.7</v>
+        <v>4.7300000000000004</v>
       </c>
       <c r="F24">
-        <v>11.4</v>
+        <v>15.3</v>
       </c>
       <c r="G24" t="s">
         <v>14</v>
@@ -2012,10 +1998,10 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <v>0.749</v>
-      </c>
-      <c r="L24" s="1">
-        <v>2.1399999999999999E-2</v>
+        <v>0.747</v>
+      </c>
+      <c r="L24">
+        <v>5.8799999999999998E-2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -2050,9 +2036,9 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>0.749</v>
-      </c>
-      <c r="L25" s="1">
+        <v>0.746</v>
+      </c>
+      <c r="L25">
         <v>0</v>
       </c>
     </row>
@@ -2067,7 +2053,7 @@
         <v>971</v>
       </c>
       <c r="D26">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -2085,13 +2071,13 @@
         <v>14</v>
       </c>
       <c r="J26">
-        <v>3.9899999999999998E-2</v>
+        <v>4.41E-2</v>
       </c>
       <c r="K26">
-        <v>0.748</v>
+        <v>0.752</v>
       </c>
       <c r="L26">
-        <v>0.88</v>
+        <v>0.83099999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>